<commit_message>
Fixed stock proce data not to have nan values in the first period
</commit_message>
<xml_diff>
--- a/Financial Modelling Prep Library/Company Financial Data/NVDA/quarter/stock_price_data.xlsx
+++ b/Financial Modelling Prep Library/Company Financial Data/NVDA/quarter/stock_price_data.xlsx
@@ -467,6 +467,15 @@
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B2">
+        <v>60.83499908447266</v>
+      </c>
+      <c r="C2">
+        <v>45.14500045776367</v>
+      </c>
+      <c r="D2">
+        <v>52.18639355018491</v>
+      </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">

</xml_diff>